<commit_message>
update the bounds for double down strategy
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,15 +16,14 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">                       position level
-take profit</t>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,16 +31,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -49,24 +61,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color auto="1"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>